<commit_message>
add LCOA scenario for RTLM prioritisation
</commit_message>
<xml_diff>
--- a/2_outputs/tables/scenarios_results.xlsx
+++ b/2_outputs/tables/scenarios_results.xlsx
@@ -617,35 +617,35 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CET ($65.8) + Demand constraint + Drug budget + Donor constraint</t>
+          <t>CET ($164.7) + Demand constraint + Drug budget + HR constraint</t>
         </is>
       </c>
       <c r="B8">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C8">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D8">
-        <v>44241794.11</v>
+        <v>64412836.83</v>
       </c>
       <c r="E8">
-        <v>2064.552864</v>
+        <v>152.79</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.9892513549003035</v>
       </c>
       <c r="G8">
-        <v>1.63</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>0.51</v>
+        <v>0.43</v>
       </c>
       <c r="I8">
-        <v>1.54</v>
+        <v>0.85</v>
       </c>
       <c r="J8">
-        <v>0.06</v>
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>
@@ -709,19 +709,19 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>CET ($65.8) + Demand constraint + Drug budget + Donor constraint</t>
+          <t>CET ($164.7) + Demand constraint + Drug budget + HR constraint</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Child Health</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>002</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Child Health</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -748,18 +748,18 @@
         <v>0.4699999999999922</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.4699999999999921</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Child Health</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>007</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Child Health</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -792,12 +792,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Child Health</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>010</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Child Health</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -830,12 +830,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Child Health</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>012</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Child Health</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -862,18 +862,18 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.7100000000004439</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Child Health</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>027</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Child Health</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -906,12 +906,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Child Health</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>028</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Child Health</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -938,18 +938,18 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.1358508743601793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Child Health</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>029</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Child Health</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -976,18 +976,18 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.9999999999993293</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Eye, Ear and Skin</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>044</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Eye, Ear and Skin</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1020,14 +1020,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Eye, Ear and Skin</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>057</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Eye, Ear and Skin</t>
-        </is>
-      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>Trachoma mass drug administration</t>
@@ -1052,18 +1052,18 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>0.6999999999999998</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>061</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1090,18 +1090,18 @@
         <v>1.000000000000037</v>
       </c>
       <c r="J11">
-        <v>0.2264181239336322</v>
+        <v>1.000000000000037</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>062</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1128,18 +1128,18 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.203776311540269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>063</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1166,18 +1166,18 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0.203776311540269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>065</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1210,12 +1210,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>066</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1248,12 +1248,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>069</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1286,12 +1286,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>070</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1324,12 +1324,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>077</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1356,18 +1356,18 @@
         <v>0.4</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>078</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1394,20 +1394,20 @@
         <v>0.5999999999999999</v>
       </c>
       <c r="J19">
-        <v>0.1358508743601793</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>079</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
-        </is>
-      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>Condom promotion among key populations (Female sex workers)</t>
@@ -1432,20 +1432,20 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0.1358508743601793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>080</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
-        </is>
-      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>Condom promotion among key populations (MSM)</t>
@@ -1470,18 +1470,18 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.1358508743601793</v>
+        <v>0.6000000000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>081</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1508,20 +1508,20 @@
         <v>0.25</v>
       </c>
       <c r="J22">
-        <v>0.05660453098340804</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>082</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
-        </is>
-      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>IDU: needle exchange</t>
@@ -1546,20 +1546,20 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0.05660453098340804</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>083</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
-        </is>
-      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>Methadone maintenance treatment (MMT) programme among injection drug users (IDUs)</t>
@@ -1584,18 +1584,18 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0.05660453098340804</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>085</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1628,12 +1628,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>086</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1660,18 +1660,18 @@
         <v>0.9000000000000001</v>
       </c>
       <c r="J26">
-        <v>0.203776311540269</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>088</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1704,12 +1704,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>089</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1742,12 +1742,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>091</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1780,12 +1780,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>092</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1812,20 +1812,20 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="J30">
-        <v>0.1584926867535425</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>093</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
-        </is>
-      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>HIV Behaviour change intervention (Schools - 10-18 years)</t>
@@ -1850,18 +1850,18 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0.1584926867535425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>094</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1888,18 +1888,18 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>0.9999999999996588</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>095</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1932,12 +1932,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>096</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1964,18 +1964,18 @@
         <v>0.6000000000001343</v>
       </c>
       <c r="J34">
-        <v>0.6000000000001344</v>
+        <v>0.6000000000001343</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>097</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2002,18 +2002,18 @@
         <v>0.6000000000002146</v>
       </c>
       <c r="J35">
-        <v>0.6000000000002145</v>
+        <v>0.6000000000002146</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>100</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2040,18 +2040,18 @@
         <v>0.5999999999999478</v>
       </c>
       <c r="J36">
-        <v>0.5999999999999479</v>
+        <v>0.5999999999999478</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>HIV/AIDS</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>101</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>HIV/AIDS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2084,12 +2084,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>Malaria</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>105</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Malaria</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2116,20 +2116,20 @@
         <v>0.95</v>
       </c>
       <c r="J38">
-        <v>0.2150972177369506</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>Malaria</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>107</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Malaria</t>
-        </is>
-      </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>IPT (pregnant women)</t>
@@ -2154,18 +2154,18 @@
         <v>0</v>
       </c>
       <c r="J39">
-        <v>0.2150972177369506</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>Malaria</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>108</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Malaria</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2192,18 +2192,18 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>0.1811344991469057</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>Malaria</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>116</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Malaria</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2230,18 +2230,18 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>0.1811344991469057</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>Malaria</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>117</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Malaria</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2268,18 +2268,18 @@
         <v>0</v>
       </c>
       <c r="J42">
-        <v>0.1811344991469057</v>
+        <v>0.8000000000000136</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>Malaria</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>125</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Malaria</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2306,18 +2306,18 @@
         <v>0.9999999999994367</v>
       </c>
       <c r="J43">
-        <v>0.2264181239336322</v>
+        <v>0.9999999999994368</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>127</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2350,12 +2350,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>130</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2382,20 +2382,20 @@
         <v>0.9499999999999998</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>0.9499999999999997</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>131</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
-        </is>
-      </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>Daily iron and folic acid supplementation (pregnant women)</t>
@@ -2420,18 +2420,18 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
           <t>132</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2464,12 +2464,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
           <t>133</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2496,18 +2496,18 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>0.9499999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>Malaria</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
           <t>134</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Malaria</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2540,12 +2540,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>135</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2572,18 +2572,18 @@
         <v>0.6000000000001127</v>
       </c>
       <c r="J50">
-        <v>0.1358508743601793</v>
+        <v>0.6000000000001128</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>136</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2610,18 +2610,18 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>0.1584926867535425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>137</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2654,12 +2654,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>138</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2686,18 +2686,18 @@
         <v>0.5674760449961503</v>
       </c>
       <c r="J53">
-        <v>0.1358508743601793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>139</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2724,18 +2724,18 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>0.1358508743601793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>140</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2762,18 +2762,18 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>0.1358508743601793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>141</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2800,18 +2800,18 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>0.599999999999744</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>142</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2838,18 +2838,18 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>0.6000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>143</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2876,18 +2876,18 @@
         <v>0.5000000000003846</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>0.5000000000003847</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>144</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2914,18 +2914,18 @@
         <v>0</v>
       </c>
       <c r="J59">
-        <v>0</v>
+        <v>0.8000000000006154</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
           <t>145</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2952,18 +2952,18 @@
         <v>0.05</v>
       </c>
       <c r="J60">
-        <v>0.05</v>
+        <v>0.05000000000000001</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
           <t>146</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2996,12 +2996,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
           <t>147</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3034,12 +3034,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
           <t>148</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3066,18 +3066,18 @@
         <v>0.9499999999999997</v>
       </c>
       <c r="J63">
-        <v>0.95</v>
+        <v>0.9500000000000001</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
           <t>149</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3110,12 +3110,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
           <t>150</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3142,18 +3142,18 @@
         <v>0.9499999999993445</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>0.9499999999993444</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
           <t>151</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3180,18 +3180,18 @@
         <v>0.9499999999994823</v>
       </c>
       <c r="J66">
-        <v>0.06603378316286558</v>
+        <v>0.9499999999994824</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
           <t>152</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3218,18 +3218,18 @@
         <v>0.95</v>
       </c>
       <c r="J67">
-        <v>0.9500000000000001</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
           <t>154</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3262,12 +3262,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>156</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3294,18 +3294,18 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
           <t>158</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3332,18 +3332,18 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>0.9500000000004774</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
           <t>160</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3370,18 +3370,18 @@
         <v>0.9499999999997759</v>
       </c>
       <c r="J71">
-        <v>0.9499999999997761</v>
+        <v>0.9499999999997762</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
           <t>163</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3414,12 +3414,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
           <t>164</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3452,12 +3452,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>165</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3490,12 +3490,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
           <t>168</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3528,12 +3528,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
           <t>169</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3566,12 +3566,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
+          <t>Maternal/Newborn and Reproductive Health</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
           <t>170</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Maternal/Newborn and Reproductive Health</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3604,12 +3604,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
+          <t>Mental, Neurological and Substance use disorders</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
           <t>173</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Mental, Neurological and Substance use disorders</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3642,12 +3642,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>Mental, Neurological and Substance use disorders</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
           <t>175</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Mental, Neurological and Substance use disorders</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3680,12 +3680,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
+          <t>Mental, Neurological and Substance use disorders</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
           <t>176</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Mental, Neurological and Substance use disorders</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3718,12 +3718,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>Mental, Neurological and Substance use disorders</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
           <t>178</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Mental, Neurological and Substance use disorders</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3750,18 +3750,18 @@
         <v>0</v>
       </c>
       <c r="J81">
-        <v>0</v>
+        <v>0.6000000000002113</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>Mental, Neurological and Substance use disorders</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
           <t>179</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Mental, Neurological and Substance use disorders</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3794,12 +3794,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
+          <t>Mental, Neurological and Substance use disorders</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
           <t>181</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Mental, Neurological and Substance use disorders</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3832,12 +3832,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>Mental, Neurological and Substance use disorders</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
           <t>185</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Mental, Neurological and Substance use disorders</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3870,12 +3870,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
+          <t>Mental, Neurological and Substance use disorders</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
           <t>187</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Mental, Neurological and Substance use disorders</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3908,14 +3908,14 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
+          <t>Neglected Tropical Disease</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
           <t>191</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Neglected Tropical Disease</t>
-        </is>
-      </c>
       <c r="C86" t="inlineStr">
         <is>
           <t>Schistosomiasis mass drug administration (adults)</t>
@@ -3940,18 +3940,18 @@
         <v>0</v>
       </c>
       <c r="J86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
+          <t>Neglected Tropical Disease</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
           <t>192</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Neglected Tropical Disease</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3984,12 +3984,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
           <t>198</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -4022,12 +4022,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
           <t>199</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -4060,12 +4060,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
           <t>204</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -4098,12 +4098,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
           <t>210</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -4130,18 +4130,18 @@
         <v>0</v>
       </c>
       <c r="J91">
-        <v>0</v>
+        <v>0.9000000000006638</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
           <t>211</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -4174,12 +4174,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
           <t>213</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -4212,12 +4212,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
           <t>216</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4250,12 +4250,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
           <t>219</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4282,18 +4282,18 @@
         <v>0</v>
       </c>
       <c r="J95">
-        <v>0.1584926867535425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
           <t>220</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4320,18 +4320,18 @@
         <v>0</v>
       </c>
       <c r="J96">
-        <v>0.1132090619668161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
           <t>226</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4364,12 +4364,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
           <t>227</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4402,12 +4402,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
           <t>228</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4440,12 +4440,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
           <t>229</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4472,18 +4472,18 @@
         <v>0.9999999999994605</v>
       </c>
       <c r="J100">
-        <v>0.9999999999994605</v>
+        <v>0.9999999999994607</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
           <t>230</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -4510,18 +4510,18 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>0.5000000000002506</v>
+        <v>0.2005600796501301</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
           <t>231</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -4554,12 +4554,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
           <t>232</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -4592,12 +4592,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
           <t>233</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4624,18 +4624,18 @@
         <v>0.899999999999798</v>
       </c>
       <c r="J104">
-        <v>0.899999999999798</v>
+        <v>0.8999999999997979</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
+          <t>Non-Communicable Disease and Injury</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
           <t>234</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Non-Communicable Disease and Injury</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -4668,12 +4668,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
           <t>236</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -4706,12 +4706,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
           <t>237</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4738,18 +4738,18 @@
         <v>0</v>
       </c>
       <c r="J107">
-        <v>0.203776311540269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
           <t>241</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -4782,12 +4782,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
           <t>243</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -4814,18 +4814,18 @@
         <v>0</v>
       </c>
       <c r="J109">
-        <v>0.203776311540269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
           <t>245</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -4858,12 +4858,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
           <t>248</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4896,12 +4896,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
           <t>250</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4934,12 +4934,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
           <t>251</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4972,12 +4972,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
           <t>257</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -5004,18 +5004,18 @@
         <v>0.9499999999999997</v>
       </c>
       <c r="J114">
-        <v>0.95</v>
+        <v>0.9500000000000001</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
+          <t>Respiratory disease including COVID-19</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
           <t>279</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Respiratory disease including COVID-19</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -5048,12 +5048,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
+          <t>Respiratory disease including COVID-19</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
           <t>280</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Respiratory disease including COVID-19</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -5086,12 +5086,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
+          <t>Respiratory disease including COVID-19</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
           <t>282</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Respiratory disease including COVID-19</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -5124,12 +5124,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
+          <t>Respiratory disease including COVID-19</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
           <t>283</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Respiratory disease including COVID-19</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -5162,12 +5162,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
+          <t>Respiratory disease including COVID-19</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
           <t>284</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Respiratory disease including COVID-19</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -5200,12 +5200,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
+          <t>Respiratory disease including COVID-19</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
           <t>290</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>Respiratory disease including COVID-19</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -5238,12 +5238,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
+          <t>Respiratory disease including COVID-19</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
           <t>291</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>Respiratory disease including COVID-19</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -5276,12 +5276,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
+          <t>Tuberculosis</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
           <t>298</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -5308,20 +5308,20 @@
         <v>0</v>
       </c>
       <c r="J122">
-        <v>0.203776311540269</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
+          <t>Tuberculosis</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
           <t>299</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
-        </is>
-      </c>
       <c r="C123" t="inlineStr">
         <is>
           <t>Targeted Xpert for patients with presumptive tuberculosis (Smear negative, HIV positive, retreatment, contacts of MDR-TB cases)</t>
@@ -5346,18 +5346,18 @@
         <v>0</v>
       </c>
       <c r="J123">
-        <v>0.203776311540269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
+          <t>Tuberculosis</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
           <t>307</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -5384,18 +5384,18 @@
         <v>0.92</v>
       </c>
       <c r="J124">
-        <v>0.9199999999999999</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
+          <t>Tuberculosis</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
           <t>308</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -5428,12 +5428,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
+          <t>Tuberculosis</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
           <t>309</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -5466,12 +5466,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
+          <t>Tuberculosis</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
           <t>310</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -5498,20 +5498,20 @@
         <v>0.8</v>
       </c>
       <c r="J127">
-        <v>0.1811344991469057</v>
+        <v>0.7999999999999998</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
+          <t>Tuberculosis</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
           <t>311</t>
         </is>
       </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
-        </is>
-      </c>
       <c r="C128" t="inlineStr">
         <is>
           <t>Full DOTS (smear-positive, smear negative and Extrapulmonary cases)</t>
@@ -5536,18 +5536,18 @@
         <v>0</v>
       </c>
       <c r="J128">
-        <v>0.1811344991469057</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
+          <t>Vaccine Preventable Disease</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
           <t>322</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>Vaccine Preventable Disease</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -5574,20 +5574,20 @@
         <v>0</v>
       </c>
       <c r="J129">
-        <v>0.2218897614549595</v>
+        <v>0.9800000000000001</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
+          <t>Vaccine Preventable Disease</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
           <t>323</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>Vaccine Preventable Disease</t>
-        </is>
-      </c>
       <c r="C130" t="inlineStr">
         <is>
           <t>Polio vaccine</t>
@@ -5612,20 +5612,20 @@
         <v>0</v>
       </c>
       <c r="J130">
-        <v>0.2173613989762869</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
+          <t>Vaccine Preventable Disease</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
           <t>324</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>Vaccine Preventable Disease</t>
-        </is>
-      </c>
       <c r="C131" t="inlineStr">
         <is>
           <t>BCG vaccine</t>
@@ -5650,20 +5650,20 @@
         <v>0</v>
       </c>
       <c r="J131">
-        <v>0.2264181239336322</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
+          <t>Vaccine Preventable Disease</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
           <t>325</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>Vaccine Preventable Disease</t>
-        </is>
-      </c>
       <c r="C132" t="inlineStr">
         <is>
           <t>Pneumococcal vaccine</t>
@@ -5688,18 +5688,18 @@
         <v>0</v>
       </c>
       <c r="J132">
-        <v>0.2196255802156232</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
+          <t>Vaccine Preventable Disease</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
           <t>326</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>Vaccine Preventable Disease</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -5732,12 +5732,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
+          <t>Vaccine Preventable Disease</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
           <t>328</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>Vaccine Preventable Disease</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -5764,18 +5764,18 @@
         <v>0.9799999999999999</v>
       </c>
       <c r="J134">
-        <v>0.2218897614549595</v>
+        <v>0.9800000000000001</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
+          <t>Vaccine Preventable Disease</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
           <t>329</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Vaccine Preventable Disease</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -5802,18 +5802,18 @@
         <v>0</v>
       </c>
       <c r="J135">
-        <v>0.2218897614549595</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
+          <t>Vaccine Preventable Disease</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
           <t>331</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>Vaccine Preventable Disease</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -5846,12 +5846,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
+          <t>Child Health</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
           <t>333</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>Child Health</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -5878,18 +5878,18 @@
         <v>0</v>
       </c>
       <c r="J137">
-        <v>0</v>
+        <v>0.8000000000001412</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
           <t>347</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -5916,20 +5916,20 @@
         <v>0.6000000000002502</v>
       </c>
       <c r="J138">
-        <v>0.1358508743601793</v>
+        <v>0.6000000000002502</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
           <t>348</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
-        </is>
-      </c>
       <c r="C139" t="inlineStr">
         <is>
           <t>Sugar fortification with vitamin-A</t>
@@ -5954,18 +5954,18 @@
         <v>0</v>
       </c>
       <c r="J139">
-        <v>0</v>
+        <v>0.6000000000000001</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
           <t>349</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -5992,18 +5992,18 @@
         <v>0.5900000000000001</v>
       </c>
       <c r="J140">
-        <v>0</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
           <t>350</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -6036,12 +6036,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
           <t>351</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">

</xml_diff>

<commit_message>
add scenario 9 - Lomas CET + Demand + Drug budget
</commit_message>
<xml_diff>
--- a/2_outputs/tables/scenarios_results.xlsx
+++ b/2_outputs/tables/scenarios_results.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -648,6 +648,40 @@
         <v>0.21</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CET ($164.7) + Demand constraint + Drug budget</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>89</v>
+      </c>
+      <c r="C9">
+        <v>72</v>
+      </c>
+      <c r="D9">
+        <v>67918104.11</v>
+      </c>
+      <c r="E9">
+        <v>123.64</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2.98</v>
+      </c>
+      <c r="H9">
+        <v>1.52</v>
+      </c>
+      <c r="I9">
+        <v>4.56</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -655,7 +689,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J142"/>
+  <dimension ref="A1:K142"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -712,6 +746,11 @@
           <t>CET ($164.7) + Demand constraint + Drug budget + HR constraint</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>CET ($164.7) + Demand constraint + Drug budget</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -750,6 +789,9 @@
       <c r="J2">
         <v>0.4699999999999921</v>
       </c>
+      <c r="K2">
+        <v>0.4699999999999921</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -788,6 +830,9 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -826,6 +871,9 @@
       <c r="J4">
         <v>0</v>
       </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -864,6 +912,9 @@
       <c r="J5">
         <v>0.7100000000004439</v>
       </c>
+      <c r="K5">
+        <v>0.7100000000004439</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -902,6 +953,9 @@
       <c r="J6">
         <v>0</v>
       </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -940,6 +994,9 @@
       <c r="J7">
         <v>0</v>
       </c>
+      <c r="K7">
+        <v>0.5999999999998817</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -978,6 +1035,9 @@
       <c r="J8">
         <v>0.9999999999993293</v>
       </c>
+      <c r="K8">
+        <v>0.9999999999993293</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1016,6 +1076,9 @@
       <c r="J9">
         <v>0.4699999999997057</v>
       </c>
+      <c r="K9">
+        <v>0.4699999999997057</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1054,6 +1117,9 @@
       <c r="J10">
         <v>0.6999999999999998</v>
       </c>
+      <c r="K10">
+        <v>0.6999999999999998</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1092,6 +1158,9 @@
       <c r="J11">
         <v>1.000000000000037</v>
       </c>
+      <c r="K11">
+        <v>1.000000000000037</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1130,6 +1199,9 @@
       <c r="J12">
         <v>0</v>
       </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1168,6 +1240,9 @@
       <c r="J13">
         <v>0</v>
       </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1206,6 +1281,9 @@
       <c r="J14">
         <v>0</v>
       </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1244,6 +1322,9 @@
       <c r="J15">
         <v>0</v>
       </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1282,6 +1363,9 @@
       <c r="J16">
         <v>0</v>
       </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1320,6 +1404,9 @@
       <c r="J17">
         <v>0</v>
       </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1358,6 +1445,9 @@
       <c r="J18">
         <v>0.4</v>
       </c>
+      <c r="K18">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1396,6 +1486,9 @@
       <c r="J19">
         <v>0.6</v>
       </c>
+      <c r="K19">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1434,6 +1527,9 @@
       <c r="J20">
         <v>0</v>
       </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1472,6 +1568,9 @@
       <c r="J21">
         <v>0.6000000000000001</v>
       </c>
+      <c r="K21">
+        <v>0.6000000000000001</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1510,6 +1609,9 @@
       <c r="J22">
         <v>0.25</v>
       </c>
+      <c r="K22">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1548,6 +1650,9 @@
       <c r="J23">
         <v>0</v>
       </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1586,6 +1691,9 @@
       <c r="J24">
         <v>0</v>
       </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1624,6 +1732,9 @@
       <c r="J25">
         <v>1</v>
       </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1662,6 +1773,9 @@
       <c r="J26">
         <v>0.8999999999999999</v>
       </c>
+      <c r="K26">
+        <v>0.8999999999999999</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1700,6 +1814,9 @@
       <c r="J27">
         <v>0</v>
       </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1738,6 +1855,9 @@
       <c r="J28">
         <v>0</v>
       </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1776,6 +1896,9 @@
       <c r="J29">
         <v>0</v>
       </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1814,6 +1937,9 @@
       <c r="J30">
         <v>0.7</v>
       </c>
+      <c r="K30">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1852,6 +1978,9 @@
       <c r="J31">
         <v>0</v>
       </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1890,6 +2019,9 @@
       <c r="J32">
         <v>0.9999999999996588</v>
       </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1928,6 +2060,9 @@
       <c r="J33">
         <v>0</v>
       </c>
+      <c r="K33">
+        <v>0.9000000000000001</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1966,6 +2101,9 @@
       <c r="J34">
         <v>0.6000000000001343</v>
       </c>
+      <c r="K34">
+        <v>0.6000000000001343</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2004,6 +2142,9 @@
       <c r="J35">
         <v>0.6000000000002146</v>
       </c>
+      <c r="K35">
+        <v>0.6000000000002146</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2042,6 +2183,9 @@
       <c r="J36">
         <v>0.5999999999999478</v>
       </c>
+      <c r="K36">
+        <v>0.5999999999999478</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2080,6 +2224,9 @@
       <c r="J37">
         <v>0.899999999999381</v>
       </c>
+      <c r="K37">
+        <v>0.899999999999381</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2118,6 +2265,9 @@
       <c r="J38">
         <v>0.95</v>
       </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2156,6 +2306,9 @@
       <c r="J39">
         <v>0</v>
       </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2194,6 +2347,9 @@
       <c r="J40">
         <v>0</v>
       </c>
+      <c r="K40">
+        <v>0.799999999999664</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2232,6 +2388,9 @@
       <c r="J41">
         <v>0</v>
       </c>
+      <c r="K41">
+        <v>0.800000000000141</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2270,6 +2429,9 @@
       <c r="J42">
         <v>0.8000000000000136</v>
       </c>
+      <c r="K42">
+        <v>0.8000000000000136</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2308,6 +2470,9 @@
       <c r="J43">
         <v>0.9999999999994368</v>
       </c>
+      <c r="K43">
+        <v>0.9999999999994368</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2346,6 +2511,9 @@
       <c r="J44">
         <v>0</v>
       </c>
+      <c r="K44">
+        <v>0.622495157119452</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2384,6 +2552,9 @@
       <c r="J45">
         <v>0.9499999999999997</v>
       </c>
+      <c r="K45">
+        <v>0.9499999999999997</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2422,6 +2593,9 @@
       <c r="J46">
         <v>0.95</v>
       </c>
+      <c r="K46">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2460,6 +2634,9 @@
       <c r="J47">
         <v>0</v>
       </c>
+      <c r="K47">
+        <v>0.9499999999999998</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2498,6 +2675,9 @@
       <c r="J48">
         <v>0</v>
       </c>
+      <c r="K48">
+        <v>0.9499999999999997</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2536,6 +2716,9 @@
       <c r="J49">
         <v>0.5999999999998286</v>
       </c>
+      <c r="K49">
+        <v>0.5999999999998286</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2574,6 +2757,9 @@
       <c r="J50">
         <v>0.6000000000001128</v>
       </c>
+      <c r="K50">
+        <v>0.6000000000001128</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2612,6 +2798,9 @@
       <c r="J51">
         <v>0</v>
       </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2650,6 +2839,9 @@
       <c r="J52">
         <v>0</v>
       </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2688,6 +2880,9 @@
       <c r="J53">
         <v>0</v>
       </c>
+      <c r="K53">
+        <v>0.5999999999996756</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2726,6 +2921,9 @@
       <c r="J54">
         <v>0</v>
       </c>
+      <c r="K54">
+        <v>0.5999999999999488</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2764,6 +2962,9 @@
       <c r="J55">
         <v>0</v>
       </c>
+      <c r="K55">
+        <v>0.6000000000001128</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2802,6 +3003,9 @@
       <c r="J56">
         <v>0</v>
       </c>
+      <c r="K56">
+        <v>0.599999999999744</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2840,6 +3044,9 @@
       <c r="J57">
         <v>0</v>
       </c>
+      <c r="K57">
+        <v>0.6000000000000002</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2878,6 +3085,9 @@
       <c r="J58">
         <v>0.5000000000003847</v>
       </c>
+      <c r="K58">
+        <v>0.5000000000003847</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2916,6 +3126,9 @@
       <c r="J59">
         <v>0.8000000000006154</v>
       </c>
+      <c r="K59">
+        <v>0.8000000000006154</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2954,6 +3167,9 @@
       <c r="J60">
         <v>0.05000000000000001</v>
       </c>
+      <c r="K60">
+        <v>0.05000000000000001</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2992,6 +3208,9 @@
       <c r="J61">
         <v>0</v>
       </c>
+      <c r="K61">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3030,6 +3249,9 @@
       <c r="J62">
         <v>0</v>
       </c>
+      <c r="K62">
+        <v>0.9500000000002184</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3068,6 +3290,9 @@
       <c r="J63">
         <v>0.9500000000000001</v>
       </c>
+      <c r="K63">
+        <v>0.9500000000000001</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3106,6 +3331,9 @@
       <c r="J64">
         <v>0</v>
       </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3144,6 +3372,9 @@
       <c r="J65">
         <v>0.9499999999993444</v>
       </c>
+      <c r="K65">
+        <v>0.9499999999993444</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3182,6 +3413,9 @@
       <c r="J66">
         <v>0.9499999999994824</v>
       </c>
+      <c r="K66">
+        <v>0.9499999999994824</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3220,6 +3454,9 @@
       <c r="J67">
         <v>0.95</v>
       </c>
+      <c r="K67">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3258,6 +3495,9 @@
       <c r="J68">
         <v>0</v>
       </c>
+      <c r="K68">
+        <v>0.9500000000004576</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3296,6 +3536,9 @@
       <c r="J69">
         <v>0</v>
       </c>
+      <c r="K69">
+        <v>0.9499999999999998</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3334,6 +3577,9 @@
       <c r="J70">
         <v>0</v>
       </c>
+      <c r="K70">
+        <v>0.9500000000004774</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3372,6 +3618,9 @@
       <c r="J71">
         <v>0.9499999999997762</v>
       </c>
+      <c r="K71">
+        <v>0.9499999999997762</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3410,6 +3659,9 @@
       <c r="J72">
         <v>0</v>
       </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3448,6 +3700,9 @@
       <c r="J73">
         <v>0</v>
       </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3486,6 +3741,9 @@
       <c r="J74">
         <v>0</v>
       </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3524,6 +3782,9 @@
       <c r="J75">
         <v>0.9499999999994906</v>
       </c>
+      <c r="K75">
+        <v>0.9499999999994906</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3562,6 +3823,9 @@
       <c r="J76">
         <v>0.95</v>
       </c>
+      <c r="K76">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3600,6 +3864,9 @@
       <c r="J77">
         <v>0.95</v>
       </c>
+      <c r="K77">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3638,6 +3905,9 @@
       <c r="J78">
         <v>0</v>
       </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3676,6 +3946,9 @@
       <c r="J79">
         <v>0</v>
       </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3714,6 +3987,9 @@
       <c r="J80">
         <v>0</v>
       </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3752,6 +4028,9 @@
       <c r="J81">
         <v>0.6000000000002113</v>
       </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3790,6 +4069,9 @@
       <c r="J82">
         <v>0</v>
       </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3828,6 +4110,9 @@
       <c r="J83">
         <v>0</v>
       </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3866,6 +4151,9 @@
       <c r="J84">
         <v>0</v>
       </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3904,6 +4192,9 @@
       <c r="J85">
         <v>0</v>
       </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3942,6 +4233,9 @@
       <c r="J86">
         <v>1</v>
       </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3980,6 +4274,9 @@
       <c r="J87">
         <v>1</v>
       </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4018,6 +4315,9 @@
       <c r="J88">
         <v>0</v>
       </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4056,6 +4356,9 @@
       <c r="J89">
         <v>0</v>
       </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4094,6 +4397,9 @@
       <c r="J90">
         <v>0</v>
       </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4132,6 +4438,9 @@
       <c r="J91">
         <v>0.9000000000006638</v>
       </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4170,6 +4479,9 @@
       <c r="J92">
         <v>0</v>
       </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4208,6 +4520,9 @@
       <c r="J93">
         <v>0</v>
       </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4246,6 +4561,9 @@
       <c r="J94">
         <v>0</v>
       </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4284,6 +4602,9 @@
       <c r="J95">
         <v>0</v>
       </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4322,6 +4643,9 @@
       <c r="J96">
         <v>0</v>
       </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4360,6 +4684,9 @@
       <c r="J97">
         <v>0</v>
       </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4398,6 +4725,9 @@
       <c r="J98">
         <v>0</v>
       </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4436,6 +4766,9 @@
       <c r="J99">
         <v>0</v>
       </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4474,6 +4807,9 @@
       <c r="J100">
         <v>0.9999999999994607</v>
       </c>
+      <c r="K100">
+        <v>0.9999999999994607</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4512,6 +4848,9 @@
       <c r="J101">
         <v>0.2005600796501301</v>
       </c>
+      <c r="K101">
+        <v>0.5000000000002506</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4550,6 +4889,9 @@
       <c r="J102">
         <v>0</v>
       </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4588,6 +4930,9 @@
       <c r="J103">
         <v>0</v>
       </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4626,6 +4971,9 @@
       <c r="J104">
         <v>0.8999999999997979</v>
       </c>
+      <c r="K104">
+        <v>0.8999999999997979</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4664,6 +5012,9 @@
       <c r="J105">
         <v>0</v>
       </c>
+      <c r="K105">
+        <v>0.5000000000001524</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4702,6 +5053,9 @@
       <c r="J106">
         <v>0</v>
       </c>
+      <c r="K106">
+        <v>0.9399999999999999</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4740,6 +5094,9 @@
       <c r="J107">
         <v>0</v>
       </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4778,6 +5135,9 @@
       <c r="J108">
         <v>0</v>
       </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4816,6 +5176,9 @@
       <c r="J109">
         <v>0</v>
       </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4854,6 +5217,9 @@
       <c r="J110">
         <v>0</v>
       </c>
+      <c r="K110">
+        <v>0.9400000000000002</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4892,6 +5258,9 @@
       <c r="J111">
         <v>0</v>
       </c>
+      <c r="K111">
+        <v>0.9399999999999999</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4930,6 +5299,9 @@
       <c r="J112">
         <v>0</v>
       </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4968,6 +5340,9 @@
       <c r="J113">
         <v>0</v>
       </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5006,6 +5381,9 @@
       <c r="J114">
         <v>0.9500000000000001</v>
       </c>
+      <c r="K114">
+        <v>0.9500000000000001</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5044,6 +5422,9 @@
       <c r="J115">
         <v>0</v>
       </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5082,6 +5463,9 @@
       <c r="J116">
         <v>0</v>
       </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5120,6 +5504,9 @@
       <c r="J117">
         <v>0</v>
       </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5158,6 +5545,9 @@
       <c r="J118">
         <v>0</v>
       </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5196,6 +5586,9 @@
       <c r="J119">
         <v>0</v>
       </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5234,6 +5627,9 @@
       <c r="J120">
         <v>0</v>
       </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5272,6 +5668,9 @@
       <c r="J121">
         <v>0</v>
       </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5310,6 +5709,9 @@
       <c r="J122">
         <v>0.9</v>
       </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5348,6 +5750,9 @@
       <c r="J123">
         <v>0</v>
       </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5386,6 +5791,9 @@
       <c r="J124">
         <v>0.92</v>
       </c>
+      <c r="K124">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5424,6 +5832,9 @@
       <c r="J125">
         <v>0</v>
       </c>
+      <c r="K125">
+        <v>0.5999999999999999</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5462,6 +5873,9 @@
       <c r="J126">
         <v>0.92</v>
       </c>
+      <c r="K126">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5500,6 +5914,9 @@
       <c r="J127">
         <v>0.7999999999999998</v>
       </c>
+      <c r="K127">
+        <v>0.7999999999999998</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5538,6 +5955,9 @@
       <c r="J128">
         <v>0</v>
       </c>
+      <c r="K128">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5576,6 +5996,9 @@
       <c r="J129">
         <v>0.9800000000000001</v>
       </c>
+      <c r="K129">
+        <v>0.9800000000000001</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5614,6 +6037,9 @@
       <c r="J130">
         <v>0</v>
       </c>
+      <c r="K130">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5652,6 +6078,9 @@
       <c r="J131">
         <v>1</v>
       </c>
+      <c r="K131">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5690,6 +6119,9 @@
       <c r="J132">
         <v>0.97</v>
       </c>
+      <c r="K132">
+        <v>0.97</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5728,6 +6160,9 @@
       <c r="J133">
         <v>0</v>
       </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5766,6 +6201,9 @@
       <c r="J134">
         <v>0.9800000000000001</v>
       </c>
+      <c r="K134">
+        <v>0.9800000000000001</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5804,6 +6242,9 @@
       <c r="J135">
         <v>0</v>
       </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5842,6 +6283,9 @@
       <c r="J136">
         <v>0</v>
       </c>
+      <c r="K136">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5880,6 +6324,9 @@
       <c r="J137">
         <v>0.8000000000001412</v>
       </c>
+      <c r="K137">
+        <v>0.8000000000001412</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5918,6 +6365,9 @@
       <c r="J138">
         <v>0.6000000000002502</v>
       </c>
+      <c r="K138">
+        <v>0.6000000000002502</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5956,6 +6406,9 @@
       <c r="J139">
         <v>0.6000000000000001</v>
       </c>
+      <c r="K139">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5994,6 +6447,9 @@
       <c r="J140">
         <v>0.59</v>
       </c>
+      <c r="K140">
+        <v>0.59</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -6032,6 +6488,9 @@
       <c r="J141">
         <v>0</v>
       </c>
+      <c r="K141">
+        <v>0</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -6068,6 +6527,9 @@
         <v>0</v>
       </c>
       <c r="J142">
+        <v>0</v>
+      </c>
+      <c r="K142">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
convert donor constraint analysis into a function
</commit_message>
<xml_diff>
--- a/2_outputs/tables/scenarios_results.xlsx
+++ b/2_outputs/tables/scenarios_results.xlsx
@@ -748,7 +748,7 @@
         <v>0.4699999999999922</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.4699999999999921</v>
       </c>
     </row>
     <row r="3">
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="8">
@@ -1090,7 +1090,7 @@
         <v>1.000000000000037</v>
       </c>
       <c r="J11">
-        <v>0.2264181239336322</v>
+        <v>0.2689990491248384</v>
       </c>
     </row>
     <row r="12">
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0.203776311540269</v>
+        <v>0.2420991442123545</v>
       </c>
     </row>
     <row r="13">
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0.203776311540269</v>
+        <v>0.2420991442123545</v>
       </c>
     </row>
     <row r="14">
@@ -1356,7 +1356,7 @@
         <v>0.4</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>0.4000000000000001</v>
       </c>
     </row>
     <row r="19">
@@ -1394,7 +1394,7 @@
         <v>0.5999999999999999</v>
       </c>
       <c r="J19">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="20">
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="21">
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="22">
@@ -1508,7 +1508,7 @@
         <v>0.25</v>
       </c>
       <c r="J22">
-        <v>0.05660453098340804</v>
+        <v>0.06724976228120959</v>
       </c>
     </row>
     <row r="23">
@@ -1546,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0.05660453098340804</v>
+        <v>0.06724976228120959</v>
       </c>
     </row>
     <row r="24">
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0.05660453098340804</v>
+        <v>0.06724976228120959</v>
       </c>
     </row>
     <row r="25">
@@ -1660,7 +1660,7 @@
         <v>0.9000000000000001</v>
       </c>
       <c r="J26">
-        <v>0.203776311540269</v>
+        <v>0.2420991442123545</v>
       </c>
     </row>
     <row r="27">
@@ -1812,7 +1812,7 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="J30">
-        <v>0.1584926867535425</v>
+        <v>0.1882993343873868</v>
       </c>
     </row>
     <row r="31">
@@ -1850,7 +1850,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0.1584926867535425</v>
+        <v>0.1882993343873868</v>
       </c>
     </row>
     <row r="32">
@@ -2116,7 +2116,7 @@
         <v>0.95</v>
       </c>
       <c r="J38">
-        <v>0.2150972177369506</v>
+        <v>0.2555490966685964</v>
       </c>
     </row>
     <row r="39">
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="J39">
-        <v>0.2150972177369506</v>
+        <v>0.2555490966685964</v>
       </c>
     </row>
     <row r="40">
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>0.1811344991469057</v>
+        <v>0.2151992392998707</v>
       </c>
     </row>
     <row r="41">
@@ -2230,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>0.1811344991469057</v>
+        <v>0.2151992392998707</v>
       </c>
     </row>
     <row r="42">
@@ -2268,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="J42">
-        <v>0.1811344991469057</v>
+        <v>0.2151992392998707</v>
       </c>
     </row>
     <row r="43">
@@ -2306,7 +2306,7 @@
         <v>0.9999999999994367</v>
       </c>
       <c r="J43">
-        <v>0.2264181239336322</v>
+        <v>0.2689990491248384</v>
       </c>
     </row>
     <row r="44">
@@ -2382,7 +2382,7 @@
         <v>0.9499999999999998</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>0.9499999999999997</v>
       </c>
     </row>
     <row r="46">
@@ -2572,7 +2572,7 @@
         <v>0.6000000000001127</v>
       </c>
       <c r="J50">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="51">
@@ -2610,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>0.1584926867535425</v>
+        <v>0.1882993343873868</v>
       </c>
     </row>
     <row r="52">
@@ -2686,7 +2686,7 @@
         <v>0.5674760449961503</v>
       </c>
       <c r="J53">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="54">
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="55">
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="56">
@@ -2876,7 +2876,7 @@
         <v>0.5000000000003846</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>0.5000000000003847</v>
       </c>
     </row>
     <row r="59">
@@ -3142,7 +3142,7 @@
         <v>0.9499999999993445</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>0.9499999999993445</v>
       </c>
     </row>
     <row r="66">
@@ -3180,7 +3180,7 @@
         <v>0.9499999999994823</v>
       </c>
       <c r="J66">
-        <v>0.06603378316286558</v>
+        <v>0.9499999999994823</v>
       </c>
     </row>
     <row r="67">
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>0.9500000000004774</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -4282,7 +4282,7 @@
         <v>0</v>
       </c>
       <c r="J95">
-        <v>0.1584926867535425</v>
+        <v>0.1882993343873868</v>
       </c>
     </row>
     <row r="96">
@@ -4320,7 +4320,7 @@
         <v>0</v>
       </c>
       <c r="J96">
-        <v>0.1132090619668161</v>
+        <v>0.1344995245624192</v>
       </c>
     </row>
     <row r="97">
@@ -4510,7 +4510,7 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>0.5000000000002506</v>
+        <v>0.2186871614598355</v>
       </c>
     </row>
     <row r="102">
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
       <c r="J107">
-        <v>0.203776311540269</v>
+        <v>0.2420991442123545</v>
       </c>
     </row>
     <row r="108">
@@ -4776,7 +4776,7 @@
         <v>0</v>
       </c>
       <c r="J108">
-        <v>0</v>
+        <v>0.6000000000002502</v>
       </c>
     </row>
     <row r="109">
@@ -4814,7 +4814,7 @@
         <v>0</v>
       </c>
       <c r="J109">
-        <v>0.203776311540269</v>
+        <v>0.2420991442123545</v>
       </c>
     </row>
     <row r="110">
@@ -5308,7 +5308,7 @@
         <v>0</v>
       </c>
       <c r="J122">
-        <v>0.203776311540269</v>
+        <v>0.2420991442123545</v>
       </c>
     </row>
     <row r="123">
@@ -5346,7 +5346,7 @@
         <v>0</v>
       </c>
       <c r="J123">
-        <v>0.203776311540269</v>
+        <v>0.2420991442123545</v>
       </c>
     </row>
     <row r="124">
@@ -5498,7 +5498,7 @@
         <v>0.8</v>
       </c>
       <c r="J127">
-        <v>0.1811344991469057</v>
+        <v>0.2151992392998707</v>
       </c>
     </row>
     <row r="128">
@@ -5536,7 +5536,7 @@
         <v>0</v>
       </c>
       <c r="J128">
-        <v>0.1811344991469057</v>
+        <v>0.2151992392998707</v>
       </c>
     </row>
     <row r="129">
@@ -5574,7 +5574,7 @@
         <v>0</v>
       </c>
       <c r="J129">
-        <v>0.2218897614549595</v>
+        <v>0.2636190681423416</v>
       </c>
     </row>
     <row r="130">
@@ -5612,7 +5612,7 @@
         <v>0</v>
       </c>
       <c r="J130">
-        <v>0.2173613989762869</v>
+        <v>0.2582390871598448</v>
       </c>
     </row>
     <row r="131">
@@ -5650,7 +5650,7 @@
         <v>0</v>
       </c>
       <c r="J131">
-        <v>0.2264181239336322</v>
+        <v>0.2689990491248384</v>
       </c>
     </row>
     <row r="132">
@@ -5688,7 +5688,7 @@
         <v>0</v>
       </c>
       <c r="J132">
-        <v>0.2196255802156232</v>
+        <v>0.2609290776510932</v>
       </c>
     </row>
     <row r="133">
@@ -5764,7 +5764,7 @@
         <v>0.9799999999999999</v>
       </c>
       <c r="J134">
-        <v>0.2218897614549595</v>
+        <v>0.2636190681423416</v>
       </c>
     </row>
     <row r="135">
@@ -5802,7 +5802,7 @@
         <v>0</v>
       </c>
       <c r="J135">
-        <v>0.2218897614549595</v>
+        <v>0.2636190681423416</v>
       </c>
     </row>
     <row r="136">
@@ -5916,7 +5916,7 @@
         <v>0.6000000000002502</v>
       </c>
       <c r="J138">
-        <v>0.1358508743601793</v>
+        <v>0.161399429474903</v>
       </c>
     </row>
     <row r="139">
@@ -5992,7 +5992,7 @@
         <v>0.5900000000000001</v>
       </c>
       <c r="J140">
-        <v>0</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="141">

</xml_diff>

<commit_message>
fix error in cervical cancer interventions - hr need and consumable cost
</commit_message>
<xml_diff>
--- a/2_outputs/tables/scenarios_results.xlsx
+++ b/2_outputs/tables/scenarios_results.xlsx
@@ -429,16 +429,16 @@
         <v>19470.29</v>
       </c>
       <c r="F2">
-        <v>10.68860999824887</v>
+        <v>5.709401947836266</v>
       </c>
       <c r="G2">
-        <v>5.44</v>
+        <v>5.45</v>
       </c>
       <c r="H2">
-        <v>3.28</v>
+        <v>3.26</v>
       </c>
       <c r="I2">
-        <v>8.31</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="J2">
         <v>0.48</v>
@@ -472,7 +472,7 @@
         <v>1.58</v>
       </c>
       <c r="I3">
-        <v>3.62</v>
+        <v>3.68</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -497,16 +497,16 @@
         <v>159.28</v>
       </c>
       <c r="F4">
-        <v>8.575509479827449</v>
+        <v>3.596301429414845</v>
       </c>
       <c r="G4">
-        <v>4.48</v>
+        <v>4.49</v>
       </c>
       <c r="H4">
-        <v>2.17</v>
+        <v>2.2</v>
       </c>
       <c r="I4">
-        <v>7.22</v>
+        <v>6.87</v>
       </c>
       <c r="J4">
         <v>0.23</v>
@@ -540,7 +540,7 @@
         <v>1.29</v>
       </c>
       <c r="I5">
-        <v>2.81</v>
+        <v>2.79</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -574,7 +574,7 @@
         <v>1.23</v>
       </c>
       <c r="I6">
-        <v>2.51</v>
+        <v>2.49</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -605,10 +605,10 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.42</v>
+        <v>0.43</v>
       </c>
       <c r="I7">
-        <v>0.73</v>
+        <v>0.6</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -627,7 +627,7 @@
         <v>66</v>
       </c>
       <c r="D8">
-        <v>44241794.11</v>
+        <v>57214110.16</v>
       </c>
       <c r="E8">
         <v>2064.552864</v>
@@ -636,16 +636,16 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1.63</v>
+        <v>2.29</v>
       </c>
       <c r="H8">
-        <v>0.51</v>
+        <v>1.05</v>
       </c>
       <c r="I8">
-        <v>1.54</v>
+        <v>3.51</v>
       </c>
       <c r="J8">
-        <v>0.06</v>
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>
@@ -733,19 +733,19 @@
         <v>0.9999999999999832</v>
       </c>
       <c r="E2">
-        <v>0.9999999999999836</v>
+        <v>0.9999999999999833</v>
       </c>
       <c r="F2">
         <v>0.9999999999999833</v>
       </c>
       <c r="G2">
-        <v>0.4699999999999922</v>
+        <v>0.4699999999999921</v>
       </c>
       <c r="H2">
-        <v>0.4699999999999922</v>
+        <v>0.4699999999999921</v>
       </c>
       <c r="I2">
-        <v>0.4699999999999922</v>
+        <v>0.4699999999999921</v>
       </c>
       <c r="J2">
         <v>0.4699999999999921</v>
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.9999999999998028</v>
+        <v>0.9999999999998029</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.9999999999999835</v>
+        <v>0.9999999999999831</v>
       </c>
       <c r="E6">
         <v>0.9999999999999833</v>
@@ -891,10 +891,10 @@
         <v>0.9999999999999832</v>
       </c>
       <c r="G6">
-        <v>0.6999999999999883</v>
+        <v>0.6999999999999882</v>
       </c>
       <c r="H6">
-        <v>0.5265700766604371</v>
+        <v>0.5265700766604366</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9999999999998027</v>
+        <v>0.999999999999803</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -958,7 +958,7 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9999999999993293</v>
+        <v>0.9999999999993295</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -996,22 +996,22 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.9999999999993737</v>
+        <v>0.9999999999993738</v>
       </c>
       <c r="E9">
         <v>0.9999999999993737</v>
       </c>
       <c r="F9">
-        <v>0.9999999999993738</v>
+        <v>0.9999999999993739</v>
       </c>
       <c r="G9">
-        <v>0.4699999999997057</v>
+        <v>0.4699999999997056</v>
       </c>
       <c r="H9">
-        <v>0.4699999999997057</v>
+        <v>0.4699999999997056</v>
       </c>
       <c r="I9">
-        <v>0.4699999999997057</v>
+        <v>0.4699999999997056</v>
       </c>
       <c r="J9">
         <v>0.4699999999997057</v>
@@ -1224,7 +1224,7 @@
         </is>
       </c>
       <c r="D15">
-        <v>0.447630235258813</v>
+        <v>0.4476302352588128</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="D16">
-        <v>0.4999999999996715</v>
+        <v>0.4999999999996716</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="D17">
-        <v>0.999999999999343</v>
+        <v>0.9999999999993427</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="D18">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1379,19 +1379,19 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19">
-        <v>0.5999999999999999</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="H19">
-        <v>0.5999999999999999</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="I19">
-        <v>0.5999999999999999</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="J19">
         <v>0.161399429474903</v>
@@ -1528,7 +1528,7 @@
         </is>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1651,13 +1651,13 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <v>0.9000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="H26">
-        <v>0.9000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="I26">
-        <v>0.9000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="J26">
         <v>0.2420991442123545</v>
@@ -1680,7 +1680,7 @@
         </is>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1803,13 +1803,13 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <v>0.7000000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="H30">
-        <v>0.7000000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="I30">
-        <v>0.7000000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="J30">
         <v>0.1882993343873868</v>
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="D32">
-        <v>0.9999999999996588</v>
+        <v>0.9999999999996589</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -2022,22 +2022,22 @@
         </is>
       </c>
       <c r="D36">
+        <v>0.9999999999999133</v>
+      </c>
+      <c r="E36">
         <v>0.9999999999999132</v>
       </c>
-      <c r="E36">
-        <v>0.9999999999999131</v>
-      </c>
       <c r="F36">
-        <v>0.9999999999999132</v>
+        <v>0.999999999999913</v>
       </c>
       <c r="G36">
-        <v>0.5999999999999478</v>
+        <v>0.5999999999999479</v>
       </c>
       <c r="H36">
-        <v>0.5999999999999478</v>
+        <v>0.5999999999999479</v>
       </c>
       <c r="I36">
-        <v>0.5999999999999478</v>
+        <v>0.5999999999999479</v>
       </c>
       <c r="J36">
         <v>0.5999999999999479</v>
@@ -2063,19 +2063,19 @@
         <v>0.9999999999993123</v>
       </c>
       <c r="E37">
-        <v>0.9999999999993122</v>
+        <v>0.9999999999993121</v>
       </c>
       <c r="F37">
-        <v>0.9999999999993122</v>
+        <v>0.9999999999993123</v>
       </c>
       <c r="G37">
-        <v>0.899999999999381</v>
+        <v>0.8999999999993809</v>
       </c>
       <c r="H37">
-        <v>0.899999999999381</v>
+        <v>0.8999999999993809</v>
       </c>
       <c r="I37">
-        <v>0.899999999999381</v>
+        <v>0.8999999999993809</v>
       </c>
       <c r="J37">
         <v>0.899999999999381</v>
@@ -2107,13 +2107,13 @@
         <v>1</v>
       </c>
       <c r="G38">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="J38">
         <v>0.2555490966685964</v>
@@ -2136,7 +2136,7 @@
         </is>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2174,13 +2174,13 @@
         </is>
       </c>
       <c r="D40">
+        <v>0.99999999999958</v>
+      </c>
+      <c r="E40">
+        <v>0.99999999999958</v>
+      </c>
+      <c r="F40">
         <v>0.9999999999995799</v>
-      </c>
-      <c r="E40">
-        <v>0.9999999999995799</v>
-      </c>
-      <c r="F40">
-        <v>0.99999999999958</v>
       </c>
       <c r="G40">
         <v>0.799999999999664</v>
@@ -2218,13 +2218,13 @@
         <v>1.000000000000177</v>
       </c>
       <c r="F41">
-        <v>1.000000000000177</v>
+        <v>1.000000000000176</v>
       </c>
       <c r="G41">
-        <v>0.8000000000001413</v>
+        <v>0.8000000000001412</v>
       </c>
       <c r="H41">
-        <v>0.8000000000001413</v>
+        <v>0.8000000000001412</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -2294,7 +2294,7 @@
         <v>0.9999999999994367</v>
       </c>
       <c r="F43">
-        <v>0.9999999999994368</v>
+        <v>0.9999999999994366</v>
       </c>
       <c r="G43">
         <v>0.9999999999994367</v>
@@ -2326,7 +2326,7 @@
         </is>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2367,19 +2367,19 @@
         <v>1</v>
       </c>
       <c r="E45">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>0.9499999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="H45">
-        <v>0.9499999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="I45">
-        <v>0.9499999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="J45">
         <v>0.9499999999999997</v>
@@ -2478,19 +2478,19 @@
         </is>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G48">
-        <v>0.9500000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="H48">
-        <v>0.9500000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -2519,7 +2519,7 @@
         <v>0.9999999999997142</v>
       </c>
       <c r="E49">
-        <v>0.9999999999997139</v>
+        <v>0.9999999999997141</v>
       </c>
       <c r="F49">
         <v>0.9999999999997141</v>
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="D51">
-        <v>1.000000000000544</v>
+        <v>1.000000000000545</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2668,22 +2668,22 @@
         </is>
       </c>
       <c r="D53">
-        <v>0.9999999999994593</v>
+        <v>0.9999999999994594</v>
       </c>
       <c r="E53">
-        <v>0.9999999999994592</v>
+        <v>0.9999999999994594</v>
       </c>
       <c r="F53">
         <v>0.9999999999994593</v>
       </c>
       <c r="G53">
-        <v>0.5999999999996756</v>
+        <v>0.5999999999996757</v>
       </c>
       <c r="H53">
-        <v>0.5999999999996756</v>
+        <v>0.5999999999996757</v>
       </c>
       <c r="I53">
-        <v>0.5674760449961503</v>
+        <v>0.5674760449961508</v>
       </c>
       <c r="J53">
         <v>0.161399429474903</v>
@@ -2706,19 +2706,19 @@
         </is>
       </c>
       <c r="D54">
+        <v>0.9999999999999147</v>
+      </c>
+      <c r="E54">
+        <v>0.9999999999999147</v>
+      </c>
+      <c r="F54">
         <v>0.9999999999999145</v>
       </c>
-      <c r="E54">
-        <v>0.9999999999999148</v>
-      </c>
-      <c r="F54">
-        <v>0.9999999999999146</v>
-      </c>
       <c r="G54">
-        <v>0.5999999999999489</v>
+        <v>0.5999999999999488</v>
       </c>
       <c r="H54">
-        <v>0.5999999999999489</v>
+        <v>0.5999999999999488</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -2782,19 +2782,19 @@
         </is>
       </c>
       <c r="D56">
-        <v>0.9999999999995733</v>
+        <v>0.9999999999995732</v>
       </c>
       <c r="E56">
-        <v>0.9999999999995732</v>
+        <v>0.9999999999995731</v>
       </c>
       <c r="F56">
         <v>0.9999999999995731</v>
       </c>
       <c r="G56">
-        <v>0.599999999999744</v>
+        <v>0.5999999999997438</v>
       </c>
       <c r="H56">
-        <v>0.599999999999744</v>
+        <v>0.5999999999997438</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -2829,10 +2829,10 @@
         <v>1</v>
       </c>
       <c r="G57">
-        <v>0.6000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="H57">
-        <v>0.6000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -2867,13 +2867,13 @@
         <v>1.000000000000769</v>
       </c>
       <c r="G58">
-        <v>0.5000000000003846</v>
+        <v>0.5000000000003847</v>
       </c>
       <c r="H58">
-        <v>0.5000000000003846</v>
+        <v>0.5000000000003847</v>
       </c>
       <c r="I58">
-        <v>0.5000000000003846</v>
+        <v>0.5000000000003847</v>
       </c>
       <c r="J58">
         <v>0.5000000000003847</v>
@@ -2943,13 +2943,13 @@
         <v>1</v>
       </c>
       <c r="G60">
-        <v>0.05</v>
+        <v>0.05000000000000001</v>
       </c>
       <c r="H60">
-        <v>0.05</v>
+        <v>0.05000000000000001</v>
       </c>
       <c r="I60">
-        <v>0.05</v>
+        <v>0.05000000000000001</v>
       </c>
       <c r="J60">
         <v>0.05</v>
@@ -2975,16 +2975,16 @@
         <v>1</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="G61">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="H61">
-        <v>0.95</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -3019,10 +3019,10 @@
         <v>1.00000000000023</v>
       </c>
       <c r="G62">
-        <v>0.9500000000002184</v>
+        <v>0.9500000000002186</v>
       </c>
       <c r="H62">
-        <v>0.9500000000002184</v>
+        <v>0.9500000000002186</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -3057,13 +3057,13 @@
         <v>1</v>
       </c>
       <c r="G63">
-        <v>0.9499999999999997</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="H63">
-        <v>0.9499999999999997</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="I63">
-        <v>0.9499999999999997</v>
+        <v>0.9499999999999998</v>
       </c>
       <c r="J63">
         <v>0.95</v>
@@ -3095,10 +3095,10 @@
         <v>1</v>
       </c>
       <c r="G64">
-        <v>0.9500000000000002</v>
+        <v>0.95</v>
       </c>
       <c r="H64">
-        <v>0.9500000000000002</v>
+        <v>0.95</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -3127,7 +3127,7 @@
         <v>0.99999999999931</v>
       </c>
       <c r="E65">
-        <v>0.9999999999993098</v>
+        <v>0.9999999999993099</v>
       </c>
       <c r="F65">
         <v>0.9999999999993099</v>
@@ -3139,7 +3139,7 @@
         <v>0.9499999999993443</v>
       </c>
       <c r="I65">
-        <v>0.9499999999993445</v>
+        <v>0.9499999999993443</v>
       </c>
       <c r="J65">
         <v>0.9499999999993445</v>
@@ -3168,7 +3168,7 @@
         <v>0.999999999999455</v>
       </c>
       <c r="F66">
-        <v>0.9999999999994552</v>
+        <v>0.9999999999994551</v>
       </c>
       <c r="G66">
         <v>0.9499999999994823</v>
@@ -3200,7 +3200,7 @@
         </is>
       </c>
       <c r="D67">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -3247,10 +3247,10 @@
         <v>1.000000000000482</v>
       </c>
       <c r="G68">
-        <v>0.9500000000004577</v>
+        <v>0.9500000000004578</v>
       </c>
       <c r="H68">
-        <v>0.9500000000004577</v>
+        <v>0.9500000000004578</v>
       </c>
       <c r="I68">
         <v>0</v>
@@ -3282,7 +3282,7 @@
         <v>1</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G69">
         <v>0.95</v>
@@ -3352,22 +3352,22 @@
         </is>
       </c>
       <c r="D71">
-        <v>0.9999999999997646</v>
+        <v>0.9999999999997643</v>
       </c>
       <c r="E71">
+        <v>0.9999999999997644</v>
+      </c>
+      <c r="F71">
         <v>0.9999999999997642</v>
       </c>
-      <c r="F71">
-        <v>0.9999999999997645</v>
-      </c>
       <c r="G71">
-        <v>0.9499999999997759</v>
+        <v>0.9499999999997761</v>
       </c>
       <c r="H71">
-        <v>0.9499999999997759</v>
+        <v>0.9499999999997761</v>
       </c>
       <c r="I71">
-        <v>0.9499999999997759</v>
+        <v>0.9499999999997761</v>
       </c>
       <c r="J71">
         <v>0.9499999999997761</v>
@@ -3504,13 +3504,13 @@
         </is>
       </c>
       <c r="D75">
+        <v>0.9999999999994639</v>
+      </c>
+      <c r="E75">
+        <v>0.9999999999994637</v>
+      </c>
+      <c r="F75">
         <v>0.9999999999994638</v>
-      </c>
-      <c r="E75">
-        <v>0.9999999999994638</v>
-      </c>
-      <c r="F75">
-        <v>0.9999999999994639</v>
       </c>
       <c r="G75">
         <v>0.9499999999994905</v>
@@ -3586,16 +3586,16 @@
         <v>1</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G77">
-        <v>0.9499999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="H77">
-        <v>0.9499999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="I77">
-        <v>0.9499999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="J77">
         <v>0.95</v>
@@ -3656,7 +3656,7 @@
         </is>
       </c>
       <c r="D79">
-        <v>0.9999999999996587</v>
+        <v>0.9999999999996589</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -3694,7 +3694,7 @@
         </is>
       </c>
       <c r="D80">
-        <v>0.9999999999996588</v>
+        <v>0.9999999999996587</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -3846,7 +3846,7 @@
         </is>
       </c>
       <c r="D84">
-        <v>0.9999999999998568</v>
+        <v>0.9999999999998569</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -3966,7 +3966,7 @@
         <v>1</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G87">
         <v>1</v>
@@ -4118,7 +4118,7 @@
         <v>0</v>
       </c>
       <c r="F91">
-        <v>1.000000000000737</v>
+        <v>1.000000000000738</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -4302,13 +4302,13 @@
         </is>
       </c>
       <c r="D96">
+        <v>0.9999999999997462</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
         <v>0.9999999999997463</v>
-      </c>
-      <c r="E96">
-        <v>0</v>
-      </c>
-      <c r="F96">
-        <v>0.9999999999997462</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4454,22 +4454,22 @@
         </is>
       </c>
       <c r="D100">
+        <v>0.9999999999994604</v>
+      </c>
+      <c r="E100">
+        <v>0.9999999999994607</v>
+      </c>
+      <c r="F100">
         <v>0.9999999999994605</v>
       </c>
-      <c r="E100">
-        <v>0.9999999999994605</v>
-      </c>
-      <c r="F100">
+      <c r="G100">
         <v>0.9999999999994607</v>
       </c>
-      <c r="G100">
-        <v>0.9999999999994605</v>
-      </c>
       <c r="H100">
-        <v>0.9999999999994605</v>
+        <v>0.9999999999994607</v>
       </c>
       <c r="I100">
-        <v>0.9999999999994605</v>
+        <v>0.9999999999994607</v>
       </c>
       <c r="J100">
         <v>0.9999999999994605</v>
@@ -4568,13 +4568,13 @@
         </is>
       </c>
       <c r="D103">
-        <v>2.416562011124274e-07</v>
+        <v>2.416562011974176e-07</v>
       </c>
       <c r="E103">
-        <v>2.416562013060393e-07</v>
+        <v>2.416562009798508e-07</v>
       </c>
       <c r="F103">
-        <v>2.416562010349998e-07</v>
+        <v>2.416562010902471e-07</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4606,22 +4606,22 @@
         </is>
       </c>
       <c r="D104">
-        <v>0.9999999999997752</v>
+        <v>0.9999999999997753</v>
       </c>
       <c r="E104">
         <v>0.9999999999997753</v>
       </c>
       <c r="F104">
-        <v>0.9999999999997754</v>
+        <v>0.9999999999997753</v>
       </c>
       <c r="G104">
-        <v>0.899999999999798</v>
+        <v>0.8999999999997979</v>
       </c>
       <c r="H104">
-        <v>0.899999999999798</v>
+        <v>0.8999999999997979</v>
       </c>
       <c r="I104">
-        <v>0.899999999999798</v>
+        <v>0.8999999999997979</v>
       </c>
       <c r="J104">
         <v>0.899999999999798</v>
@@ -4682,7 +4682,7 @@
         </is>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E106">
         <v>0</v>
@@ -4720,7 +4720,7 @@
         </is>
       </c>
       <c r="D107">
-        <v>0.6347349860581529</v>
+        <v>0.634734986058153</v>
       </c>
       <c r="E107">
         <v>0</v>
@@ -4796,7 +4796,7 @@
         </is>
       </c>
       <c r="D109">
-        <v>0.9999999999999569</v>
+        <v>0.9999999999999568</v>
       </c>
       <c r="E109">
         <v>0</v>
@@ -4881,10 +4881,10 @@
         <v>1</v>
       </c>
       <c r="G111">
-        <v>0.9400000000000001</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="H111">
-        <v>0.9400000000000001</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="I111">
         <v>0</v>
@@ -4989,19 +4989,19 @@
         <v>1</v>
       </c>
       <c r="E114">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F114">
         <v>1</v>
       </c>
       <c r="G114">
-        <v>0.9499999999999997</v>
+        <v>0.9500000000000002</v>
       </c>
       <c r="H114">
-        <v>0.9499999999999997</v>
+        <v>0.9500000000000002</v>
       </c>
       <c r="I114">
-        <v>0.9499999999999997</v>
+        <v>0.9500000000000002</v>
       </c>
       <c r="J114">
         <v>0.95</v>
@@ -5024,7 +5024,7 @@
         </is>
       </c>
       <c r="D115">
-        <v>0.9999999999999077</v>
+        <v>0.9999999999999076</v>
       </c>
       <c r="E115">
         <v>0</v>
@@ -5138,7 +5138,7 @@
         </is>
       </c>
       <c r="D118">
-        <v>0.9999999999996155</v>
+        <v>0.9999999999996156</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -5176,7 +5176,7 @@
         </is>
       </c>
       <c r="D119">
-        <v>0.9999999999996156</v>
+        <v>0.9999999999996158</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -5214,7 +5214,7 @@
         </is>
       </c>
       <c r="D120">
-        <v>0.9999999999997841</v>
+        <v>0.999999999999784</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -5252,7 +5252,7 @@
         </is>
       </c>
       <c r="D121">
-        <v>0.01356780306062013</v>
+        <v>0.01356780306062009</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -5290,7 +5290,7 @@
         </is>
       </c>
       <c r="D122">
-        <v>0.5</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -5445,7 +5445,7 @@
         <v>1</v>
       </c>
       <c r="E126">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="F126">
         <v>1</v>
@@ -5480,13 +5480,13 @@
         </is>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="E127">
         <v>1</v>
       </c>
       <c r="F127">
-        <v>0.9999999999999998</v>
+        <v>1</v>
       </c>
       <c r="G127">
         <v>0.8</v>
@@ -5565,10 +5565,10 @@
         <v>1</v>
       </c>
       <c r="G129">
-        <v>0.9800000000000002</v>
+        <v>0.9800000000000001</v>
       </c>
       <c r="H129">
-        <v>0.9800000000000002</v>
+        <v>0.9800000000000001</v>
       </c>
       <c r="I129">
         <v>0</v>
@@ -5749,19 +5749,19 @@
         <v>1</v>
       </c>
       <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
         <v>0.9999999999999999</v>
       </c>
-      <c r="F134">
-        <v>1</v>
-      </c>
       <c r="G134">
-        <v>0.9799999999999999</v>
+        <v>0.9800000000000001</v>
       </c>
       <c r="H134">
-        <v>0.9799999999999999</v>
+        <v>0.9800000000000001</v>
       </c>
       <c r="I134">
-        <v>0.9799999999999999</v>
+        <v>0.9800000000000001</v>
       </c>
       <c r="J134">
         <v>0.2636190681423416</v>
@@ -5787,16 +5787,16 @@
         <v>1</v>
       </c>
       <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135">
         <v>0.9999999999999999</v>
       </c>
-      <c r="F135">
-        <v>1</v>
-      </c>
       <c r="G135">
-        <v>0.9799999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="H135">
-        <v>0.9799999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="I135">
         <v>0</v>
@@ -5860,7 +5860,7 @@
         </is>
       </c>
       <c r="D137">
-        <v>1.000000000000177</v>
+        <v>1.000000000000176</v>
       </c>
       <c r="E137">
         <v>0</v>

</xml_diff>